<commit_message>
fix some remaining pandas and welly bugs
</commit_message>
<xml_diff>
--- a/tests/data/borehole/borehole_collar.xlsx
+++ b/tests/data/borehole/borehole_collar.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20366"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20396"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{971FD4BE-3A23-4E90-984D-1304C8FC13DE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE6226D0-3B71-41DA-992B-E31533D96225}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -346,12 +346,12 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -368,7 +368,7 @@
         <v>508.4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Revert "Merge remote-tracking branch 'origin/main'"
This reverts commit c0f5b6f9a044835fc1da4ef2ad22abe88545df68, reversing
changes made to 8f6cf57f4046009c740e0132b8bbba62e554b3a3.
</commit_message>
<xml_diff>
--- a/tests/data/borehole/borehole_collar.xlsx
+++ b/tests/data/borehole/borehole_collar.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20396"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20366"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE6226D0-3B71-41DA-992B-E31533D96225}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{971FD4BE-3A23-4E90-984D-1304C8FC13DE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -346,12 +346,12 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -368,7 +368,7 @@
         <v>508.4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Revert "Revert "Merge remote-tracking branch 'origin/main'""
This reverts commit 8fddbfbbbeaafa62523d3b87e2b424988ae15da3.
</commit_message>
<xml_diff>
--- a/tests/data/borehole/borehole_collar.xlsx
+++ b/tests/data/borehole/borehole_collar.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20366"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20396"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{971FD4BE-3A23-4E90-984D-1304C8FC13DE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE6226D0-3B71-41DA-992B-E31533D96225}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -346,12 +346,12 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -368,7 +368,7 @@
         <v>508.4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>

</xml_diff>